<commit_message>
adding a couple of leagues
</commit_message>
<xml_diff>
--- a/nfl_teams.xlsx
+++ b/nfl_teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime Lacroix\Desktop\nba_bets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ACC6F7-E2B4-4A44-80F3-3B333176087F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB2F00-EC69-476B-B781-2979F3023940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F65DE869-8A51-4DBD-B711-FA19C5D1AAF2}"/>
+    <workbookView xWindow="-20610" yWindow="1695" windowWidth="20730" windowHeight="11160" xr2:uid="{F65DE869-8A51-4DBD-B711-FA19C5D1AAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,13 +231,13 @@
     <t>Tennessee Titans</t>
   </si>
   <si>
-    <t>Washington Football Team</t>
-  </si>
-  <si>
     <t>OAK</t>
   </si>
   <si>
     <t>WSH</t>
+  </si>
+  <si>
+    <t>Washington</t>
   </si>
 </sst>
 </file>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EE1320-57A0-451C-9FB2-ED5B774F01FA}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -866,15 +866,15 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
         <v>67</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>